<commit_message>
complete plot.py modify 出图.xlsx
</commit_message>
<xml_diff>
--- a/榆林项目/出图.xlsx
+++ b/榆林项目/出图.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\工作\榆林项目20200826-2017年陕西省教育厅重点实验室及基地项目\干旱指数\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\python\work1\GIT\榆林项目\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8CB606E-6CAF-4BE2-8BB5-2EAE8DCA446C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E4B037A-B3E0-4C7E-8505-D6B416B270EB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20700" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>降水</t>
   </si>
@@ -93,14 +93,34 @@
     <t>MSDI3</t>
   </si>
   <si>
-    <t>corr</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>lat</t>
   </si>
   <si>
     <t>lon</t>
+  </si>
+  <si>
+    <t>Pre-MK</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Runoff-MK</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>MSDI-MK</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SRI-MK</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SPI-MK</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Corr</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -194,16 +214,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -546,32 +566,35 @@
   <dimension ref="A1:DI97"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="O7" sqref="O7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="4" max="4" width="13.875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:113" x14ac:dyDescent="0.15">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="C1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>0</v>
-      </c>
       <c r="D1" s="1" t="s">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>2</v>
+        <v>24</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>4</v>
+        <v>26</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>11</v>
@@ -601,14 +624,14 @@
         <v>19</v>
       </c>
       <c r="Q1" s="3" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:113" x14ac:dyDescent="0.15">
-      <c r="A2" s="7">
+      <c r="A2" s="5">
         <v>36.875</v>
       </c>
-      <c r="B2" s="7">
+      <c r="B2" s="5">
         <v>107.375</v>
       </c>
       <c r="C2" s="1">
@@ -658,10 +681,10 @@
       </c>
     </row>
     <row r="3" spans="1:113" x14ac:dyDescent="0.15">
-      <c r="A3" s="7">
+      <c r="A3" s="5">
         <v>36.875</v>
       </c>
-      <c r="B3" s="7">
+      <c r="B3" s="5">
         <v>107.625</v>
       </c>
       <c r="C3" s="1">
@@ -807,10 +830,10 @@
       <c r="DI3" s="2"/>
     </row>
     <row r="4" spans="1:113" x14ac:dyDescent="0.15">
-      <c r="A4" s="7">
+      <c r="A4" s="5">
         <v>36.875</v>
       </c>
-      <c r="B4" s="7">
+      <c r="B4" s="5">
         <v>110.125</v>
       </c>
       <c r="C4" s="1">
@@ -886,10 +909,10 @@
       <c r="AQ4" s="2"/>
     </row>
     <row r="5" spans="1:113" x14ac:dyDescent="0.15">
-      <c r="A5" s="7">
+      <c r="A5" s="5">
         <v>36.875</v>
       </c>
-      <c r="B5" s="7">
+      <c r="B5" s="5">
         <v>110.375</v>
       </c>
       <c r="C5" s="1">
@@ -939,10 +962,10 @@
       </c>
     </row>
     <row r="6" spans="1:113" x14ac:dyDescent="0.15">
-      <c r="A6" s="7">
+      <c r="A6" s="5">
         <v>37.125</v>
       </c>
-      <c r="B6" s="7">
+      <c r="B6" s="5">
         <v>107.375</v>
       </c>
       <c r="C6" s="1">
@@ -992,10 +1015,10 @@
       </c>
     </row>
     <row r="7" spans="1:113" x14ac:dyDescent="0.15">
-      <c r="A7" s="7">
+      <c r="A7" s="5">
         <v>37.125</v>
       </c>
-      <c r="B7" s="7">
+      <c r="B7" s="5">
         <v>107.625</v>
       </c>
       <c r="C7" s="1">
@@ -1141,10 +1164,10 @@
       <c r="DI7" s="2"/>
     </row>
     <row r="8" spans="1:113" x14ac:dyDescent="0.15">
-      <c r="A8" s="7">
+      <c r="A8" s="5">
         <v>37.125</v>
       </c>
-      <c r="B8" s="7">
+      <c r="B8" s="5">
         <v>107.875</v>
       </c>
       <c r="C8" s="1">
@@ -1290,10 +1313,10 @@
       <c r="DI8" s="2"/>
     </row>
     <row r="9" spans="1:113" x14ac:dyDescent="0.15">
-      <c r="A9" s="7">
+      <c r="A9" s="5">
         <v>37.125</v>
       </c>
-      <c r="B9" s="7">
+      <c r="B9" s="5">
         <v>108.125</v>
       </c>
       <c r="C9" s="1">
@@ -1439,10 +1462,10 @@
       <c r="DI9" s="2"/>
     </row>
     <row r="10" spans="1:113" x14ac:dyDescent="0.15">
-      <c r="A10" s="7">
+      <c r="A10" s="5">
         <v>37.125</v>
       </c>
-      <c r="B10" s="7">
+      <c r="B10" s="5">
         <v>108.375</v>
       </c>
       <c r="C10" s="1">
@@ -1588,10 +1611,10 @@
       <c r="DI10" s="2"/>
     </row>
     <row r="11" spans="1:113" x14ac:dyDescent="0.15">
-      <c r="A11" s="7">
+      <c r="A11" s="5">
         <v>37.125</v>
       </c>
-      <c r="B11" s="7">
+      <c r="B11" s="5">
         <v>108.625</v>
       </c>
       <c r="C11" s="1">
@@ -1641,10 +1664,10 @@
       </c>
     </row>
     <row r="12" spans="1:113" x14ac:dyDescent="0.15">
-      <c r="A12" s="7">
+      <c r="A12" s="5">
         <v>37.125</v>
       </c>
-      <c r="B12" s="7">
+      <c r="B12" s="5">
         <v>108.875</v>
       </c>
       <c r="C12" s="1">
@@ -1694,10 +1717,10 @@
       </c>
     </row>
     <row r="13" spans="1:113" x14ac:dyDescent="0.15">
-      <c r="A13" s="7">
+      <c r="A13" s="5">
         <v>37.125</v>
       </c>
-      <c r="B13" s="7">
+      <c r="B13" s="5">
         <v>109.875</v>
       </c>
       <c r="C13" s="1">
@@ -1747,10 +1770,10 @@
       </c>
     </row>
     <row r="14" spans="1:113" x14ac:dyDescent="0.15">
-      <c r="A14" s="7">
+      <c r="A14" s="5">
         <v>37.125</v>
       </c>
-      <c r="B14" s="7">
+      <c r="B14" s="5">
         <v>110.125</v>
       </c>
       <c r="C14" s="1">
@@ -1800,10 +1823,10 @@
       </c>
     </row>
     <row r="15" spans="1:113" x14ac:dyDescent="0.15">
-      <c r="A15" s="7">
+      <c r="A15" s="5">
         <v>37.125</v>
       </c>
-      <c r="B15" s="7">
+      <c r="B15" s="5">
         <v>110.375</v>
       </c>
       <c r="C15" s="1">
@@ -1853,10 +1876,10 @@
       </c>
     </row>
     <row r="16" spans="1:113" x14ac:dyDescent="0.15">
-      <c r="A16" s="7">
+      <c r="A16" s="5">
         <v>37.125</v>
       </c>
-      <c r="B16" s="7">
+      <c r="B16" s="5">
         <v>110.625</v>
       </c>
       <c r="C16" s="1">
@@ -1906,10 +1929,10 @@
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A17" s="7">
+      <c r="A17" s="5">
         <v>37.375</v>
       </c>
-      <c r="B17" s="7">
+      <c r="B17" s="5">
         <v>107.375</v>
       </c>
       <c r="C17" s="1">
@@ -1959,10 +1982,10 @@
       </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A18" s="7">
+      <c r="A18" s="5">
         <v>37.375</v>
       </c>
-      <c r="B18" s="7">
+      <c r="B18" s="5">
         <v>107.625</v>
       </c>
       <c r="C18" s="1">
@@ -2012,10 +2035,10 @@
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A19" s="7">
+      <c r="A19" s="5">
         <v>37.375</v>
       </c>
-      <c r="B19" s="7">
+      <c r="B19" s="5">
         <v>107.875</v>
       </c>
       <c r="C19" s="1">
@@ -2065,10 +2088,10 @@
       </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A20" s="7">
+      <c r="A20" s="5">
         <v>37.375</v>
       </c>
-      <c r="B20" s="7">
+      <c r="B20" s="5">
         <v>108.125</v>
       </c>
       <c r="C20" s="1">
@@ -2118,10 +2141,10 @@
       </c>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A21" s="7">
+      <c r="A21" s="5">
         <v>37.375</v>
       </c>
-      <c r="B21" s="7">
+      <c r="B21" s="5">
         <v>108.375</v>
       </c>
       <c r="C21" s="1">
@@ -2171,10 +2194,10 @@
       </c>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A22" s="7">
+      <c r="A22" s="5">
         <v>37.375</v>
       </c>
-      <c r="B22" s="7">
+      <c r="B22" s="5">
         <v>108.625</v>
       </c>
       <c r="C22" s="1">
@@ -2224,10 +2247,10 @@
       </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A23" s="7">
+      <c r="A23" s="5">
         <v>37.375</v>
       </c>
-      <c r="B23" s="7">
+      <c r="B23" s="5">
         <v>108.875</v>
       </c>
       <c r="C23" s="1">
@@ -2277,10 +2300,10 @@
       </c>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A24" s="7">
+      <c r="A24" s="5">
         <v>37.375</v>
       </c>
-      <c r="B24" s="7">
+      <c r="B24" s="5">
         <v>109.125</v>
       </c>
       <c r="C24" s="1">
@@ -2330,10 +2353,10 @@
       </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A25" s="7">
+      <c r="A25" s="5">
         <v>37.375</v>
       </c>
-      <c r="B25" s="7">
+      <c r="B25" s="5">
         <v>109.375</v>
       </c>
       <c r="C25" s="1">
@@ -2383,10 +2406,10 @@
       </c>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A26" s="7">
+      <c r="A26" s="5">
         <v>37.375</v>
       </c>
-      <c r="B26" s="7">
+      <c r="B26" s="5">
         <v>109.625</v>
       </c>
       <c r="C26" s="1">
@@ -2436,10 +2459,10 @@
       </c>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A27" s="7">
+      <c r="A27" s="5">
         <v>37.375</v>
       </c>
-      <c r="B27" s="7">
+      <c r="B27" s="5">
         <v>109.875</v>
       </c>
       <c r="C27" s="1">
@@ -2489,10 +2512,10 @@
       </c>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A28" s="7">
+      <c r="A28" s="5">
         <v>37.375</v>
       </c>
-      <c r="B28" s="7">
+      <c r="B28" s="5">
         <v>110.125</v>
       </c>
       <c r="C28" s="1">
@@ -2542,10 +2565,10 @@
       </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A29" s="7">
+      <c r="A29" s="5">
         <v>37.375</v>
       </c>
-      <c r="B29" s="7">
+      <c r="B29" s="5">
         <v>110.375</v>
       </c>
       <c r="C29" s="1">
@@ -2595,10 +2618,10 @@
       </c>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A30" s="7">
+      <c r="A30" s="5">
         <v>37.375</v>
       </c>
-      <c r="B30" s="7">
+      <c r="B30" s="5">
         <v>110.625</v>
       </c>
       <c r="C30" s="1">
@@ -2648,10 +2671,10 @@
       </c>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A31" s="7">
+      <c r="A31" s="5">
         <v>37.625</v>
       </c>
-      <c r="B31" s="7">
+      <c r="B31" s="5">
         <v>107.375</v>
       </c>
       <c r="C31" s="1">
@@ -2701,10 +2724,10 @@
       </c>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A32" s="7">
+      <c r="A32" s="5">
         <v>37.625</v>
       </c>
-      <c r="B32" s="7">
+      <c r="B32" s="5">
         <v>107.625</v>
       </c>
       <c r="C32" s="1">
@@ -2754,10 +2777,10 @@
       </c>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A33" s="7">
+      <c r="A33" s="5">
         <v>37.625</v>
       </c>
-      <c r="B33" s="7">
+      <c r="B33" s="5">
         <v>107.875</v>
       </c>
       <c r="C33" s="1">
@@ -2807,10 +2830,10 @@
       </c>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A34" s="7">
+      <c r="A34" s="5">
         <v>37.625</v>
       </c>
-      <c r="B34" s="7">
+      <c r="B34" s="5">
         <v>108.125</v>
       </c>
       <c r="C34" s="1">
@@ -2860,10 +2883,10 @@
       </c>
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A35" s="7">
+      <c r="A35" s="5">
         <v>37.625</v>
       </c>
-      <c r="B35" s="7">
+      <c r="B35" s="5">
         <v>108.375</v>
       </c>
       <c r="C35" s="1">
@@ -2913,10 +2936,10 @@
       </c>
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A36" s="7">
+      <c r="A36" s="5">
         <v>37.625</v>
       </c>
-      <c r="B36" s="7">
+      <c r="B36" s="5">
         <v>108.625</v>
       </c>
       <c r="C36" s="1">
@@ -2966,10 +2989,10 @@
       </c>
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A37" s="7">
+      <c r="A37" s="5">
         <v>37.625</v>
       </c>
-      <c r="B37" s="7">
+      <c r="B37" s="5">
         <v>108.875</v>
       </c>
       <c r="C37" s="1">
@@ -3019,10 +3042,10 @@
       </c>
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A38" s="7">
+      <c r="A38" s="5">
         <v>37.625</v>
       </c>
-      <c r="B38" s="7">
+      <c r="B38" s="5">
         <v>109.125</v>
       </c>
       <c r="C38" s="1">
@@ -3072,10 +3095,10 @@
       </c>
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A39" s="7">
+      <c r="A39" s="5">
         <v>37.625</v>
       </c>
-      <c r="B39" s="7">
+      <c r="B39" s="5">
         <v>109.375</v>
       </c>
       <c r="C39" s="1">
@@ -3125,10 +3148,10 @@
       </c>
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A40" s="7">
+      <c r="A40" s="5">
         <v>37.625</v>
       </c>
-      <c r="B40" s="7">
+      <c r="B40" s="5">
         <v>109.625</v>
       </c>
       <c r="C40" s="1">
@@ -3178,10 +3201,10 @@
       </c>
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A41" s="7">
+      <c r="A41" s="5">
         <v>37.625</v>
       </c>
-      <c r="B41" s="7">
+      <c r="B41" s="5">
         <v>109.875</v>
       </c>
       <c r="C41" s="1">
@@ -3231,10 +3254,10 @@
       </c>
     </row>
     <row r="42" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A42" s="7">
+      <c r="A42" s="5">
         <v>37.625</v>
       </c>
-      <c r="B42" s="7">
+      <c r="B42" s="5">
         <v>110.125</v>
       </c>
       <c r="C42" s="1">
@@ -3284,10 +3307,10 @@
       </c>
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A43" s="7">
+      <c r="A43" s="5">
         <v>37.625</v>
       </c>
-      <c r="B43" s="7">
+      <c r="B43" s="5">
         <v>110.375</v>
       </c>
       <c r="C43" s="1">
@@ -3337,10 +3360,10 @@
       </c>
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A44" s="7">
+      <c r="A44" s="5">
         <v>37.625</v>
       </c>
-      <c r="B44" s="7">
+      <c r="B44" s="5">
         <v>110.625</v>
       </c>
       <c r="C44" s="1">
@@ -3390,10 +3413,10 @@
       </c>
     </row>
     <row r="45" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A45" s="7">
+      <c r="A45" s="5">
         <v>37.625</v>
       </c>
-      <c r="B45" s="7">
+      <c r="B45" s="5">
         <v>110.875</v>
       </c>
       <c r="C45" s="1">
@@ -3443,10 +3466,10 @@
       </c>
     </row>
     <row r="46" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A46" s="7">
+      <c r="A46" s="5">
         <v>37.875</v>
       </c>
-      <c r="B46" s="7">
+      <c r="B46" s="5">
         <v>107.625</v>
       </c>
       <c r="C46" s="1">
@@ -3496,10 +3519,10 @@
       </c>
     </row>
     <row r="47" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A47" s="7">
+      <c r="A47" s="5">
         <v>37.875</v>
       </c>
-      <c r="B47" s="7">
+      <c r="B47" s="5">
         <v>107.875</v>
       </c>
       <c r="C47" s="1">
@@ -3549,10 +3572,10 @@
       </c>
     </row>
     <row r="48" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A48" s="7">
+      <c r="A48" s="5">
         <v>37.875</v>
       </c>
-      <c r="B48" s="7">
+      <c r="B48" s="5">
         <v>108.875</v>
       </c>
       <c r="C48" s="1">
@@ -3602,10 +3625,10 @@
       </c>
     </row>
     <row r="49" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A49" s="7">
+      <c r="A49" s="5">
         <v>37.875</v>
       </c>
-      <c r="B49" s="7">
+      <c r="B49" s="5">
         <v>109.125</v>
       </c>
       <c r="C49" s="1">
@@ -3655,10 +3678,10 @@
       </c>
     </row>
     <row r="50" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A50" s="7">
+      <c r="A50" s="5">
         <v>37.875</v>
       </c>
-      <c r="B50" s="7">
+      <c r="B50" s="5">
         <v>109.375</v>
       </c>
       <c r="C50" s="1">
@@ -3708,10 +3731,10 @@
       </c>
     </row>
     <row r="51" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A51" s="7">
+      <c r="A51" s="5">
         <v>37.875</v>
       </c>
-      <c r="B51" s="7">
+      <c r="B51" s="5">
         <v>109.625</v>
       </c>
       <c r="C51" s="1">
@@ -3761,10 +3784,10 @@
       </c>
     </row>
     <row r="52" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A52" s="7">
+      <c r="A52" s="5">
         <v>37.875</v>
       </c>
-      <c r="B52" s="7">
+      <c r="B52" s="5">
         <v>109.875</v>
       </c>
       <c r="C52" s="1">
@@ -3814,10 +3837,10 @@
       </c>
     </row>
     <row r="53" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A53" s="7">
+      <c r="A53" s="5">
         <v>37.875</v>
       </c>
-      <c r="B53" s="7">
+      <c r="B53" s="5">
         <v>110.125</v>
       </c>
       <c r="C53" s="1">
@@ -3867,10 +3890,10 @@
       </c>
     </row>
     <row r="54" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A54" s="7">
+      <c r="A54" s="5">
         <v>37.875</v>
       </c>
-      <c r="B54" s="7">
+      <c r="B54" s="5">
         <v>110.375</v>
       </c>
       <c r="C54" s="1">
@@ -3920,10 +3943,10 @@
       </c>
     </row>
     <row r="55" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A55" s="7">
+      <c r="A55" s="5">
         <v>37.875</v>
       </c>
-      <c r="B55" s="7">
+      <c r="B55" s="5">
         <v>110.625</v>
       </c>
       <c r="C55" s="1">
@@ -3973,10 +3996,10 @@
       </c>
     </row>
     <row r="56" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A56" s="7">
+      <c r="A56" s="5">
         <v>38.125</v>
       </c>
-      <c r="B56" s="7">
+      <c r="B56" s="5">
         <v>109.125</v>
       </c>
       <c r="C56" s="1">
@@ -4026,10 +4049,10 @@
       </c>
     </row>
     <row r="57" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A57" s="7">
+      <c r="A57" s="5">
         <v>38.125</v>
       </c>
-      <c r="B57" s="7">
+      <c r="B57" s="5">
         <v>109.375</v>
       </c>
       <c r="C57" s="1">
@@ -4079,10 +4102,10 @@
       </c>
     </row>
     <row r="58" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A58" s="7">
+      <c r="A58" s="5">
         <v>38.125</v>
       </c>
-      <c r="B58" s="7">
+      <c r="B58" s="5">
         <v>109.625</v>
       </c>
       <c r="C58" s="1">
@@ -4132,10 +4155,10 @@
       </c>
     </row>
     <row r="59" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A59" s="7">
+      <c r="A59" s="5">
         <v>38.125</v>
       </c>
-      <c r="B59" s="7">
+      <c r="B59" s="5">
         <v>109.875</v>
       </c>
       <c r="C59" s="1">
@@ -4185,10 +4208,10 @@
       </c>
     </row>
     <row r="60" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A60" s="7">
+      <c r="A60" s="5">
         <v>38.125</v>
       </c>
-      <c r="B60" s="7">
+      <c r="B60" s="5">
         <v>110.125</v>
       </c>
       <c r="C60" s="1">
@@ -4238,10 +4261,10 @@
       </c>
     </row>
     <row r="61" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A61" s="7">
+      <c r="A61" s="5">
         <v>38.125</v>
       </c>
-      <c r="B61" s="7">
+      <c r="B61" s="5">
         <v>110.375</v>
       </c>
       <c r="C61" s="1">
@@ -4291,10 +4314,10 @@
       </c>
     </row>
     <row r="62" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A62" s="7">
+      <c r="A62" s="5">
         <v>38.125</v>
       </c>
-      <c r="B62" s="7">
+      <c r="B62" s="5">
         <v>110.625</v>
       </c>
       <c r="C62" s="1">
@@ -4344,10 +4367,10 @@
       </c>
     </row>
     <row r="63" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A63" s="7">
+      <c r="A63" s="5">
         <v>38.375</v>
       </c>
-      <c r="B63" s="7">
+      <c r="B63" s="5">
         <v>109.125</v>
       </c>
       <c r="C63" s="1">
@@ -4397,10 +4420,10 @@
       </c>
     </row>
     <row r="64" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A64" s="7">
+      <c r="A64" s="5">
         <v>38.375</v>
       </c>
-      <c r="B64" s="7">
+      <c r="B64" s="5">
         <v>109.375</v>
       </c>
       <c r="C64" s="1">
@@ -4450,10 +4473,10 @@
       </c>
     </row>
     <row r="65" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A65" s="7">
+      <c r="A65" s="5">
         <v>38.375</v>
       </c>
-      <c r="B65" s="7">
+      <c r="B65" s="5">
         <v>109.625</v>
       </c>
       <c r="C65" s="1">
@@ -4503,10 +4526,10 @@
       </c>
     </row>
     <row r="66" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A66" s="7">
+      <c r="A66" s="5">
         <v>38.375</v>
       </c>
-      <c r="B66" s="7">
+      <c r="B66" s="5">
         <v>109.875</v>
       </c>
       <c r="C66" s="1">
@@ -4556,10 +4579,10 @@
       </c>
     </row>
     <row r="67" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A67" s="7">
+      <c r="A67" s="5">
         <v>38.375</v>
       </c>
-      <c r="B67" s="7">
+      <c r="B67" s="5">
         <v>110.125</v>
       </c>
       <c r="C67" s="1">
@@ -4609,10 +4632,10 @@
       </c>
     </row>
     <row r="68" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A68" s="7">
+      <c r="A68" s="5">
         <v>38.375</v>
       </c>
-      <c r="B68" s="7">
+      <c r="B68" s="5">
         <v>110.375</v>
       </c>
       <c r="C68" s="1">
@@ -4662,10 +4685,10 @@
       </c>
     </row>
     <row r="69" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A69" s="7">
+      <c r="A69" s="5">
         <v>38.375</v>
       </c>
-      <c r="B69" s="7">
+      <c r="B69" s="5">
         <v>110.625</v>
       </c>
       <c r="C69" s="1">
@@ -4715,10 +4738,10 @@
       </c>
     </row>
     <row r="70" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A70" s="7">
+      <c r="A70" s="5">
         <v>38.375</v>
       </c>
-      <c r="B70" s="7">
+      <c r="B70" s="5">
         <v>110.875</v>
       </c>
       <c r="C70" s="1">
@@ -4768,10 +4791,10 @@
       </c>
     </row>
     <row r="71" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A71" s="7">
+      <c r="A71" s="5">
         <v>38.625</v>
       </c>
-      <c r="B71" s="7">
+      <c r="B71" s="5">
         <v>109.125</v>
       </c>
       <c r="C71" s="1">
@@ -4821,10 +4844,10 @@
       </c>
     </row>
     <row r="72" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A72" s="7">
+      <c r="A72" s="5">
         <v>38.625</v>
       </c>
-      <c r="B72" s="7">
+      <c r="B72" s="5">
         <v>109.375</v>
       </c>
       <c r="C72" s="1">
@@ -4874,10 +4897,10 @@
       </c>
     </row>
     <row r="73" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A73" s="7">
+      <c r="A73" s="5">
         <v>38.625</v>
       </c>
-      <c r="B73" s="7">
+      <c r="B73" s="5">
         <v>109.625</v>
       </c>
       <c r="C73" s="1">
@@ -4927,10 +4950,10 @@
       </c>
     </row>
     <row r="74" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A74" s="7">
+      <c r="A74" s="5">
         <v>38.625</v>
       </c>
-      <c r="B74" s="7">
+      <c r="B74" s="5">
         <v>109.875</v>
       </c>
       <c r="C74" s="1">
@@ -4980,10 +5003,10 @@
       </c>
     </row>
     <row r="75" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A75" s="7">
+      <c r="A75" s="5">
         <v>38.625</v>
       </c>
-      <c r="B75" s="7">
+      <c r="B75" s="5">
         <v>110.125</v>
       </c>
       <c r="C75" s="1">
@@ -5033,10 +5056,10 @@
       </c>
     </row>
     <row r="76" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A76" s="7">
+      <c r="A76" s="5">
         <v>38.625</v>
       </c>
-      <c r="B76" s="7">
+      <c r="B76" s="5">
         <v>110.375</v>
       </c>
       <c r="C76" s="1">
@@ -5086,10 +5109,10 @@
       </c>
     </row>
     <row r="77" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A77" s="7">
+      <c r="A77" s="5">
         <v>38.625</v>
       </c>
-      <c r="B77" s="7">
+      <c r="B77" s="5">
         <v>110.625</v>
       </c>
       <c r="C77" s="1">
@@ -5139,10 +5162,10 @@
       </c>
     </row>
     <row r="78" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A78" s="7">
+      <c r="A78" s="5">
         <v>38.625</v>
       </c>
-      <c r="B78" s="7">
+      <c r="B78" s="5">
         <v>110.875</v>
       </c>
       <c r="C78" s="1">
@@ -5192,10 +5215,10 @@
       </c>
     </row>
     <row r="79" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A79" s="7">
+      <c r="A79" s="5">
         <v>38.875</v>
       </c>
-      <c r="B79" s="7">
+      <c r="B79" s="5">
         <v>109.625</v>
       </c>
       <c r="C79" s="1">
@@ -5245,10 +5268,10 @@
       </c>
     </row>
     <row r="80" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A80" s="7">
+      <c r="A80" s="5">
         <v>38.875</v>
       </c>
-      <c r="B80" s="7">
+      <c r="B80" s="5">
         <v>109.875</v>
       </c>
       <c r="C80" s="1">
@@ -5298,10 +5321,10 @@
       </c>
     </row>
     <row r="81" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A81" s="7">
+      <c r="A81" s="5">
         <v>38.875</v>
       </c>
-      <c r="B81" s="7">
+      <c r="B81" s="5">
         <v>110.125</v>
       </c>
       <c r="C81" s="1">
@@ -5351,10 +5374,10 @@
       </c>
     </row>
     <row r="82" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A82" s="7">
+      <c r="A82" s="5">
         <v>38.875</v>
       </c>
-      <c r="B82" s="7">
+      <c r="B82" s="5">
         <v>110.375</v>
       </c>
       <c r="C82" s="1">
@@ -5404,10 +5427,10 @@
       </c>
     </row>
     <row r="83" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A83" s="7">
+      <c r="A83" s="5">
         <v>38.875</v>
       </c>
-      <c r="B83" s="7">
+      <c r="B83" s="5">
         <v>110.625</v>
       </c>
       <c r="C83" s="1">
@@ -5457,10 +5480,10 @@
       </c>
     </row>
     <row r="84" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A84" s="7">
+      <c r="A84" s="5">
         <v>38.875</v>
       </c>
-      <c r="B84" s="7">
+      <c r="B84" s="5">
         <v>110.875</v>
       </c>
       <c r="C84" s="1">
@@ -5510,10 +5533,10 @@
       </c>
     </row>
     <row r="85" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A85" s="7">
+      <c r="A85" s="5">
         <v>38.875</v>
       </c>
-      <c r="B85" s="7">
+      <c r="B85" s="5">
         <v>111.125</v>
       </c>
       <c r="C85" s="1">
@@ -5563,10 +5586,10 @@
       </c>
     </row>
     <row r="86" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A86" s="7">
+      <c r="A86" s="5">
         <v>39.125</v>
       </c>
-      <c r="B86" s="7">
+      <c r="B86" s="5">
         <v>109.875</v>
       </c>
       <c r="C86" s="1">
@@ -5616,10 +5639,10 @@
       </c>
     </row>
     <row r="87" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A87" s="7">
+      <c r="A87" s="5">
         <v>39.125</v>
       </c>
-      <c r="B87" s="7">
+      <c r="B87" s="5">
         <v>110.125</v>
       </c>
       <c r="C87" s="1">
@@ -5669,10 +5692,10 @@
       </c>
     </row>
     <row r="88" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A88" s="7">
+      <c r="A88" s="5">
         <v>39.125</v>
       </c>
-      <c r="B88" s="7">
+      <c r="B88" s="5">
         <v>110.375</v>
       </c>
       <c r="C88" s="1">
@@ -5722,10 +5745,10 @@
       </c>
     </row>
     <row r="89" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A89" s="7">
+      <c r="A89" s="5">
         <v>39.125</v>
       </c>
-      <c r="B89" s="7">
+      <c r="B89" s="5">
         <v>110.625</v>
       </c>
       <c r="C89" s="1">
@@ -5775,10 +5798,10 @@
       </c>
     </row>
     <row r="90" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A90" s="7">
+      <c r="A90" s="5">
         <v>39.125</v>
       </c>
-      <c r="B90" s="7">
+      <c r="B90" s="5">
         <v>110.875</v>
       </c>
       <c r="C90" s="1">
@@ -5828,10 +5851,10 @@
       </c>
     </row>
     <row r="91" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A91" s="7">
+      <c r="A91" s="5">
         <v>39.125</v>
       </c>
-      <c r="B91" s="7">
+      <c r="B91" s="5">
         <v>111.125</v>
       </c>
       <c r="C91" s="1">
@@ -5881,10 +5904,10 @@
       </c>
     </row>
     <row r="92" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A92" s="7">
+      <c r="A92" s="5">
         <v>39.375</v>
       </c>
-      <c r="B92" s="7">
+      <c r="B92" s="5">
         <v>110.125</v>
       </c>
       <c r="C92" s="1">
@@ -5934,10 +5957,10 @@
       </c>
     </row>
     <row r="93" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A93" s="7">
+      <c r="A93" s="5">
         <v>39.375</v>
       </c>
-      <c r="B93" s="7">
+      <c r="B93" s="5">
         <v>110.375</v>
       </c>
       <c r="C93" s="1">
@@ -5987,10 +6010,10 @@
       </c>
     </row>
     <row r="94" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A94" s="7">
+      <c r="A94" s="5">
         <v>39.375</v>
       </c>
-      <c r="B94" s="7">
+      <c r="B94" s="5">
         <v>110.625</v>
       </c>
       <c r="C94" s="1">
@@ -6040,10 +6063,10 @@
       </c>
     </row>
     <row r="95" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A95" s="7">
+      <c r="A95" s="5">
         <v>39.375</v>
       </c>
-      <c r="B95" s="7">
+      <c r="B95" s="5">
         <v>110.875</v>
       </c>
       <c r="C95" s="1">
@@ -6093,10 +6116,10 @@
       </c>
     </row>
     <row r="96" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A96" s="7">
+      <c r="A96" s="5">
         <v>39.375</v>
       </c>
-      <c r="B96" s="7">
+      <c r="B96" s="5">
         <v>111.125</v>
       </c>
       <c r="C96" s="1">
@@ -6146,10 +6169,10 @@
       </c>
     </row>
     <row r="97" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A97" s="7">
+      <c r="A97" s="5">
         <v>39.625</v>
       </c>
-      <c r="B97" s="7">
+      <c r="B97" s="5">
         <v>111.125</v>
       </c>
       <c r="C97" s="1">
@@ -7690,7 +7713,7 @@
       </c>
     </row>
     <row r="9" spans="1:97" x14ac:dyDescent="0.15">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="6" t="s">
         <v>5</v>
       </c>
       <c r="B9" s="2">
@@ -7983,7 +8006,7 @@
       </c>
     </row>
     <row r="10" spans="1:97" x14ac:dyDescent="0.15">
-      <c r="A10" s="4"/>
+      <c r="A10" s="6"/>
       <c r="B10" s="2">
         <v>-0.34039643242231898</v>
       </c>
@@ -8274,7 +8297,7 @@
       </c>
     </row>
     <row r="11" spans="1:97" x14ac:dyDescent="0.15">
-      <c r="A11" s="4"/>
+      <c r="A11" s="6"/>
       <c r="B11" s="2">
         <v>-1.0334025054134</v>
       </c>
@@ -8565,7 +8588,7 @@
       </c>
     </row>
     <row r="12" spans="1:97" x14ac:dyDescent="0.15">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="7" t="s">
         <v>6</v>
       </c>
       <c r="B12">
@@ -8858,7 +8881,7 @@
       </c>
     </row>
     <row r="13" spans="1:97" x14ac:dyDescent="0.15">
-      <c r="A13" s="5"/>
+      <c r="A13" s="7"/>
       <c r="B13">
         <v>-0.43409953289993303</v>
       </c>
@@ -9149,7 +9172,7 @@
       </c>
     </row>
     <row r="14" spans="1:97" s="2" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="5"/>
+      <c r="A14" s="7"/>
       <c r="B14" s="2">
         <v>-1.0760324121320901</v>
       </c>
@@ -9440,7 +9463,7 @@
       </c>
     </row>
     <row r="15" spans="1:97" s="2" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="4" t="s">
+      <c r="A15" s="6" t="s">
         <v>7</v>
       </c>
       <c r="B15" s="2">
@@ -9733,7 +9756,7 @@
       </c>
     </row>
     <row r="16" spans="1:97" s="2" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="4"/>
+      <c r="A16" s="6"/>
       <c r="B16" s="2">
         <v>-0.50049147938483995</v>
       </c>
@@ -10024,7 +10047,7 @@
       </c>
     </row>
     <row r="17" spans="1:97" s="2" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="4"/>
+      <c r="A17" s="6"/>
       <c r="B17" s="2">
         <v>-1.2491417035557399</v>
       </c>

</xml_diff>